<commit_message>
third release, minor fixes
</commit_message>
<xml_diff>
--- a/AIPrivacyChecklist.xlsx
+++ b/AIPrivacyChecklist.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="198">
   <si>
     <t>INTRODUCTION</t>
   </si>
@@ -54,7 +54,7 @@
     </r>
   </si>
   <si>
-    <t>AI Short Privacy Checklist v0.2</t>
+    <t>AI Short Privacy Checklist v0.3</t>
   </si>
   <si>
     <t>ID</t>
@@ -84,7 +84,7 @@
     <t>Centralised AI Program and governance framework is in place.</t>
   </si>
   <si>
-    <t>Implement AI Program, or any other centralised body, should be in place to coordinate and document AI use cases within the organisation. AI usage and chatbots can easily be introduced to organisation through implementation of cheap AI Agents in departments/individuals, without oversight, leading to legal and regulatory risks.
+    <t>AI Program, or any other centralised body, should be in place to coordinate and document AI use cases within the organisation. AI usage and chatbots can easily be introduced to organisation through implementation of cheap AI Agents in departments/individuals, without oversight, leading to legal and regulatory risks.
 Consider aligning AI Management System with ISO/IEC 42001 AI management system.</t>
   </si>
   <si>
@@ -94,7 +94,7 @@
     <t>Data Governance framework is implemented.</t>
   </si>
   <si>
-    <t>Implement Data Governance framework to have centralised controls and monitoring in place to control data used in AI. Governance framework should provide guidance, policies and standards for data management, and restrictions on usage of personal data.</t>
+    <t>Data Governance framework should be in place to centrally control data used in AI. Governance framework should provide guidance, policies and standards for data management, and restrictions on usage of personal data.</t>
   </si>
   <si>
     <t>AI Act Art 10</t>
@@ -115,7 +115,7 @@
     <t>Continuous compliance review process is defined and implemented</t>
   </si>
   <si>
-    <t>Implement a process for regularly reviewing AI systems for compliance with the prohibitions, including assessments of techniques used and their potential impact on users.</t>
+    <t>Process for regularly reviewing AI systems for compliance with the prohibitions should be in place, including assessments of techniques used and their potential impact on users.</t>
   </si>
   <si>
     <t>ISO42001 6.1.2</t>
@@ -146,10 +146,19 @@
     <t>GDPR Art 35</t>
   </si>
   <si>
-    <t>DPA notifications are performed as needed.</t>
-  </si>
-  <si>
-    <t>Requirements to notify Data Protection Authorities of High risk AI systems are identified. Notifications are performed in time for all systems required.</t>
+    <t>DPA notifications are performed for high risk personal data processing activities.</t>
+  </si>
+  <si>
+    <t>DPAs are notified of high risk personal data processing activities (DPIA results in high risk activity). Notifications are performed.</t>
+  </si>
+  <si>
+    <t>DPA notifications are performed as needed for high risk AI systems.</t>
+  </si>
+  <si>
+    <t>Requirements to notify Data Protection Authorities of high risk AI systems are identified. Notifications are performed.</t>
+  </si>
+  <si>
+    <t>AI Act</t>
   </si>
   <si>
     <t>High risk AI systems are registered as required.</t>
@@ -267,10 +276,10 @@
     <t>AI Act Art 9</t>
   </si>
   <si>
-    <t>High risk AI systems are identified</t>
-  </si>
-  <si>
-    <t>High risk AI systems are identified for privacy risk and treated with extra care. High risk systems are subject to AI Act regulatory requirements.</t>
+    <t>Process for identifying high risk AI systems is in place</t>
+  </si>
+  <si>
+    <t>Process for identifying high risk AI systems should be in place. Process should run continuously to identify changing business requirements and implementations. High risk systems are subject to AI Act regulatory requirements.</t>
   </si>
   <si>
     <t>Identify if intended use falls into categories of ‘Prohibited Artificial Intelligence Practices’</t>
@@ -427,6 +436,9 @@
   </si>
   <si>
     <t>Data Processing Agreements are in place with all 3rd parties with access to personal data.</t>
+  </si>
+  <si>
+    <t>GDPR Art 28</t>
   </si>
   <si>
     <t>Contractual agreements include restrictions on  personal data usage by the service provider.</t>
@@ -499,7 +511,7 @@
     <t>Personal data should be avoided to fine-tune or train the model.</t>
   </si>
   <si>
-    <t>Identify if personal data was included in the training, validation, testing or fine+tuning the model.
+    <t>Identify if personal data was included in the training, validation, testing or fine-tuning the model.
 Organisations may train models on their own private/confidential datasets and this can include employee or customer personal data. 
 Training models on personal may cause issues, as data removal is not possible without deletion of the model. Compliance risk with GDPR should be considered.</t>
   </si>
@@ -709,7 +721,7 @@
     <t>Access to logs is restricted to those with job specific need.</t>
   </si>
   <si>
-    <t>High risk AI system logs contain records from system usage..</t>
+    <t>High risk AI system logs contain records from system usage.</t>
   </si>
   <si>
     <t>For high-risk AI systems, the logging capabilities  provide, at a minimum:
@@ -2420,7 +2432,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" ht="80.05" customHeight="1">
+    <row r="4" ht="68.05" customHeight="1">
       <c r="A4" s="16"/>
       <c r="B4" t="s" s="17">
         <v>15</v>
@@ -2510,7 +2522,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" ht="44.05" customHeight="1">
+    <row r="9" ht="56.05" customHeight="1">
       <c r="A9" s="16"/>
       <c r="B9" t="s" s="17">
         <v>15</v>
@@ -2528,7 +2540,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" ht="32.05" customHeight="1">
+    <row r="10" ht="44.05" customHeight="1">
       <c r="A10" s="16"/>
       <c r="B10" t="s" s="17">
         <v>15</v>
@@ -2546,7 +2558,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" ht="140.05" customHeight="1">
+    <row r="11" ht="32.05" customHeight="1">
       <c r="A11" s="16"/>
       <c r="B11" t="s" s="17">
         <v>15</v>
@@ -2564,7 +2576,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" ht="44.05" customHeight="1">
+    <row r="12" ht="140.05" customHeight="1">
       <c r="A12" s="16"/>
       <c r="B12" t="s" s="17">
         <v>15</v>
@@ -2579,10 +2591,10 @@
         <v>46</v>
       </c>
       <c r="F12" t="s" s="18">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" ht="56.05" customHeight="1">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" ht="68.05" customHeight="1">
       <c r="A13" s="16"/>
       <c r="B13" t="s" s="17">
         <v>15</v>
@@ -2591,13 +2603,13 @@
         <v>16</v>
       </c>
       <c r="D13" t="s" s="18">
+        <v>48</v>
+      </c>
+      <c r="E13" t="s" s="18">
+        <v>49</v>
+      </c>
+      <c r="F13" t="s" s="18">
         <v>47</v>
-      </c>
-      <c r="E13" t="s" s="18">
-        <v>47</v>
-      </c>
-      <c r="F13" t="s" s="18">
-        <v>48</v>
       </c>
     </row>
     <row r="14" ht="56.05" customHeight="1">
@@ -2609,16 +2621,16 @@
         <v>16</v>
       </c>
       <c r="D14" t="s" s="18">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E14" t="s" s="18">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F14" t="s" s="18">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" ht="44.05" customHeight="1">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" ht="56.05" customHeight="1">
       <c r="A15" s="16"/>
       <c r="B15" t="s" s="17">
         <v>15</v>
@@ -2627,13 +2639,13 @@
         <v>16</v>
       </c>
       <c r="D15" t="s" s="18">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E15" t="s" s="18">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F15" t="s" s="18">
-        <v>22</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" ht="44.05" customHeight="1">
@@ -2645,13 +2657,13 @@
         <v>16</v>
       </c>
       <c r="D16" t="s" s="18">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E16" t="s" s="18">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F16" t="s" s="18">
-        <v>54</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" ht="44.05" customHeight="1">
@@ -2668,33 +2680,33 @@
       <c r="E17" t="s" s="18">
         <v>56</v>
       </c>
-      <c r="F17" s="19"/>
-    </row>
-    <row r="18" ht="20.05" customHeight="1">
+      <c r="F17" t="s" s="18">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" ht="44.05" customHeight="1">
       <c r="A18" s="16"/>
       <c r="B18" t="s" s="17">
-        <v>57</v>
+        <v>15</v>
       </c>
       <c r="C18" t="s" s="18">
+        <v>16</v>
+      </c>
+      <c r="D18" t="s" s="18">
         <v>58</v>
       </c>
-      <c r="D18" t="s" s="18">
+      <c r="E18" t="s" s="18">
         <v>59</v>
       </c>
-      <c r="E18" t="s" s="18">
-        <v>60</v>
-      </c>
-      <c r="F18" t="s" s="18">
-        <v>61</v>
-      </c>
+      <c r="F18" s="19"/>
     </row>
     <row r="19" ht="20.05" customHeight="1">
       <c r="A19" s="16"/>
       <c r="B19" t="s" s="17">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C19" t="s" s="18">
-        <v>16</v>
+        <v>61</v>
       </c>
       <c r="D19" t="s" s="18">
         <v>62</v>
@@ -2703,142 +2715,142 @@
         <v>63</v>
       </c>
       <c r="F19" t="s" s="18">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="20" ht="92.05" customHeight="1">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" ht="20.05" customHeight="1">
       <c r="A20" s="16"/>
       <c r="B20" t="s" s="17">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C20" t="s" s="18">
         <v>16</v>
       </c>
       <c r="D20" t="s" s="18">
+        <v>65</v>
+      </c>
+      <c r="E20" t="s" s="18">
+        <v>66</v>
+      </c>
+      <c r="F20" t="s" s="18">
         <v>64</v>
       </c>
-      <c r="E20" t="s" s="18">
-        <v>65</v>
-      </c>
-      <c r="F20" s="19"/>
-    </row>
-    <row r="21" ht="44.05" customHeight="1">
+    </row>
+    <row r="21" ht="92.05" customHeight="1">
       <c r="A21" s="16"/>
       <c r="B21" t="s" s="17">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C21" t="s" s="18">
         <v>16</v>
       </c>
       <c r="D21" t="s" s="18">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E21" t="s" s="18">
-        <v>67</v>
-      </c>
-      <c r="F21" t="s" s="18">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="22" ht="56.05" customHeight="1">
+        <v>68</v>
+      </c>
+      <c r="F21" s="19"/>
+    </row>
+    <row r="22" ht="44.05" customHeight="1">
       <c r="A22" s="16"/>
       <c r="B22" t="s" s="17">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C22" t="s" s="18">
         <v>16</v>
       </c>
       <c r="D22" t="s" s="18">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E22" t="s" s="18">
-        <v>69</v>
-      </c>
-      <c r="F22" s="19"/>
-    </row>
-    <row r="23" ht="44.05" customHeight="1">
+        <v>70</v>
+      </c>
+      <c r="F22" t="s" s="18">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" ht="56.05" customHeight="1">
       <c r="A23" s="16"/>
       <c r="B23" t="s" s="17">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="C23" t="s" s="18">
         <v>16</v>
       </c>
       <c r="D23" t="s" s="18">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E23" t="s" s="18">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F23" s="19"/>
     </row>
-    <row r="24" ht="92.05" customHeight="1">
+    <row r="24" ht="44.05" customHeight="1">
       <c r="A24" s="16"/>
       <c r="B24" t="s" s="17">
-        <v>72</v>
+        <v>15</v>
       </c>
       <c r="C24" t="s" s="18">
+        <v>16</v>
+      </c>
+      <c r="D24" t="s" s="18">
         <v>73</v>
       </c>
-      <c r="D24" t="s" s="18">
+      <c r="E24" t="s" s="18">
         <v>74</v>
       </c>
-      <c r="E24" t="s" s="18">
-        <v>75</v>
-      </c>
       <c r="F24" s="19"/>
     </row>
-    <row r="25" ht="44.05" customHeight="1">
+    <row r="25" ht="92.05" customHeight="1">
       <c r="A25" s="16"/>
       <c r="B25" t="s" s="17">
+        <v>75</v>
+      </c>
+      <c r="C25" t="s" s="18">
+        <v>76</v>
+      </c>
+      <c r="D25" t="s" s="18">
+        <v>77</v>
+      </c>
+      <c r="E25" t="s" s="18">
+        <v>78</v>
+      </c>
+      <c r="F25" s="19"/>
+    </row>
+    <row r="26" ht="44.05" customHeight="1">
+      <c r="A26" s="16"/>
+      <c r="B26" t="s" s="17">
         <v>15</v>
       </c>
-      <c r="C25" t="s" s="18">
+      <c r="C26" t="s" s="18">
         <v>16</v>
       </c>
-      <c r="D25" t="s" s="18">
-        <v>76</v>
-      </c>
-      <c r="E25" t="s" s="18">
-        <v>77</v>
-      </c>
-      <c r="F25" t="s" s="18">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="26" ht="20.05" customHeight="1">
-      <c r="A26" s="16"/>
-      <c r="B26" s="20"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
-    </row>
-    <row r="27" ht="44.05" customHeight="1">
+      <c r="D26" t="s" s="18">
+        <v>79</v>
+      </c>
+      <c r="E26" t="s" s="18">
+        <v>80</v>
+      </c>
+      <c r="F26" t="s" s="18">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" ht="20.05" customHeight="1">
       <c r="A27" s="16"/>
-      <c r="B27" t="s" s="17">
-        <v>15</v>
-      </c>
-      <c r="C27" t="s" s="18">
-        <v>16</v>
-      </c>
-      <c r="D27" t="s" s="18">
-        <v>79</v>
-      </c>
-      <c r="E27" t="s" s="18">
-        <v>80</v>
-      </c>
-      <c r="F27" t="s" s="18">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="28" ht="68.05" customHeight="1">
+      <c r="B27" s="20"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+    </row>
+    <row r="28" ht="44.05" customHeight="1">
       <c r="A28" s="16"/>
       <c r="B28" t="s" s="17">
         <v>15</v>
       </c>
       <c r="C28" t="s" s="18">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D28" t="s" s="18">
         <v>82</v>
@@ -2850,7 +2862,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="29" ht="104.05" customHeight="1">
+    <row r="29" ht="68.05" customHeight="1">
       <c r="A29" s="16"/>
       <c r="B29" t="s" s="17">
         <v>15</v>
@@ -2864,73 +2876,75 @@
       <c r="E29" t="s" s="18">
         <v>86</v>
       </c>
-      <c r="F29" s="19"/>
-    </row>
-    <row r="30" ht="44.05" customHeight="1">
+      <c r="F29" t="s" s="18">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30" ht="104.05" customHeight="1">
       <c r="A30" s="16"/>
       <c r="B30" t="s" s="17">
         <v>15</v>
       </c>
       <c r="C30" t="s" s="18">
+        <v>30</v>
+      </c>
+      <c r="D30" t="s" s="18">
+        <v>88</v>
+      </c>
+      <c r="E30" t="s" s="18">
+        <v>89</v>
+      </c>
+      <c r="F30" s="19"/>
+    </row>
+    <row r="31" ht="44.05" customHeight="1">
+      <c r="A31" s="16"/>
+      <c r="B31" t="s" s="17">
+        <v>15</v>
+      </c>
+      <c r="C31" t="s" s="18">
         <v>16</v>
       </c>
-      <c r="D30" t="s" s="18">
-        <v>87</v>
-      </c>
-      <c r="E30" t="s" s="18">
-        <v>88</v>
-      </c>
-      <c r="F30" t="s" s="18">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="31" ht="20.05" customHeight="1">
-      <c r="A31" s="16"/>
-      <c r="B31" s="20"/>
-      <c r="C31" s="19"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="19"/>
-    </row>
-    <row r="32" ht="44.05" customHeight="1">
+      <c r="D31" t="s" s="18">
+        <v>90</v>
+      </c>
+      <c r="E31" t="s" s="18">
+        <v>91</v>
+      </c>
+      <c r="F31" t="s" s="18">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" ht="20.05" customHeight="1">
       <c r="A32" s="16"/>
-      <c r="B32" t="s" s="17">
-        <v>57</v>
-      </c>
-      <c r="C32" t="s" s="18">
-        <v>16</v>
-      </c>
-      <c r="D32" t="s" s="18">
-        <v>90</v>
-      </c>
-      <c r="E32" t="s" s="18">
-        <v>91</v>
-      </c>
+      <c r="B32" s="20"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="19"/>
       <c r="F32" s="19"/>
     </row>
-    <row r="33" ht="116.05" customHeight="1">
+    <row r="33" ht="44.05" customHeight="1">
       <c r="A33" s="16"/>
       <c r="B33" t="s" s="17">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C33" t="s" s="18">
         <v>16</v>
       </c>
       <c r="D33" t="s" s="18">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E33" t="s" s="18">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F33" s="19"/>
     </row>
-    <row r="34" ht="32.05" customHeight="1">
+    <row r="34" ht="116.05" customHeight="1">
       <c r="A34" s="16"/>
       <c r="B34" t="s" s="17">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="C34" t="s" s="18">
-        <v>94</v>
+        <v>16</v>
       </c>
       <c r="D34" t="s" s="18">
         <v>95</v>
@@ -2940,199 +2954,211 @@
       </c>
       <c r="F34" s="19"/>
     </row>
-    <row r="35" ht="92.05" customHeight="1">
+    <row r="35" ht="32.05" customHeight="1">
       <c r="A35" s="16"/>
       <c r="B35" t="s" s="17">
         <v>15</v>
       </c>
       <c r="C35" t="s" s="18">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D35" t="s" s="18">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E35" t="s" s="18">
-        <v>98</v>
-      </c>
-      <c r="F35" s="19"/>
-    </row>
-    <row r="36" ht="56.05" customHeight="1">
+        <v>99</v>
+      </c>
+      <c r="F35" t="s" s="18">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" ht="92.05" customHeight="1">
       <c r="A36" s="16"/>
       <c r="B36" t="s" s="17">
         <v>15</v>
       </c>
       <c r="C36" t="s" s="18">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D36" t="s" s="18">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E36" t="s" s="18">
+        <v>102</v>
+      </c>
+      <c r="F36" t="s" s="18">
         <v>100</v>
       </c>
-      <c r="F36" s="19"/>
-    </row>
-    <row r="37" ht="20.05" customHeight="1">
+    </row>
+    <row r="37" ht="56.05" customHeight="1">
       <c r="A37" s="16"/>
-      <c r="B37" s="20"/>
-      <c r="C37" s="19"/>
-      <c r="D37" s="19"/>
-      <c r="E37" s="19"/>
+      <c r="B37" t="s" s="17">
+        <v>15</v>
+      </c>
+      <c r="C37" t="s" s="18">
+        <v>97</v>
+      </c>
+      <c r="D37" t="s" s="18">
+        <v>103</v>
+      </c>
+      <c r="E37" t="s" s="18">
+        <v>104</v>
+      </c>
       <c r="F37" s="19"/>
     </row>
-    <row r="38" ht="200.05" customHeight="1">
+    <row r="38" ht="20.05" customHeight="1">
       <c r="A38" s="16"/>
-      <c r="B38" t="s" s="17">
-        <v>72</v>
-      </c>
-      <c r="C38" t="s" s="18">
-        <v>101</v>
-      </c>
-      <c r="D38" t="s" s="18">
-        <v>102</v>
-      </c>
-      <c r="E38" t="s" s="18">
-        <v>103</v>
-      </c>
+      <c r="B38" s="20"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="19"/>
       <c r="F38" s="19"/>
     </row>
-    <row r="39" ht="140.05" customHeight="1">
+    <row r="39" ht="200.05" customHeight="1">
       <c r="A39" s="16"/>
       <c r="B39" t="s" s="17">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C39" t="s" s="18">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="D39" t="s" s="18">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E39" t="s" s="18">
-        <v>105</v>
-      </c>
-      <c r="F39" t="s" s="18">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="40" ht="116.05" customHeight="1">
+        <v>107</v>
+      </c>
+      <c r="F39" s="19"/>
+    </row>
+    <row r="40" ht="140.05" customHeight="1">
       <c r="A40" s="16"/>
       <c r="B40" t="s" s="17">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C40" t="s" s="18">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="D40" t="s" s="18">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E40" t="s" s="18">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F40" t="s" s="18">
         <v>22</v>
       </c>
     </row>
-    <row r="41" ht="20.05" customHeight="1">
+    <row r="41" ht="116.05" customHeight="1">
       <c r="A41" s="16"/>
-      <c r="B41" s="20"/>
-      <c r="C41" s="19"/>
-      <c r="D41" s="19"/>
-      <c r="E41" s="19"/>
-      <c r="F41" s="19"/>
+      <c r="B41" t="s" s="17">
+        <v>75</v>
+      </c>
+      <c r="C41" t="s" s="18">
+        <v>105</v>
+      </c>
+      <c r="D41" t="s" s="18">
+        <v>110</v>
+      </c>
+      <c r="E41" t="s" s="18">
+        <v>111</v>
+      </c>
+      <c r="F41" t="s" s="18">
+        <v>22</v>
+      </c>
     </row>
     <row r="42" ht="68.05" customHeight="1">
       <c r="A42" s="16"/>
       <c r="B42" t="s" s="17">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C42" t="s" s="18">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="D42" t="s" s="18">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="E42" t="s" s="18">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="F42" s="19"/>
     </row>
     <row r="43" ht="44.05" customHeight="1">
       <c r="A43" s="16"/>
       <c r="B43" t="s" s="17">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C43" t="s" s="18">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="D43" t="s" s="18">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="E43" t="s" s="18">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="F43" s="19"/>
     </row>
     <row r="44" ht="92.05" customHeight="1">
       <c r="A44" s="16"/>
       <c r="B44" t="s" s="17">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C44" t="s" s="18">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="D44" t="s" s="18">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="E44" t="s" s="18">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="F44" s="19"/>
     </row>
     <row r="45" ht="80.05" customHeight="1">
       <c r="A45" s="16"/>
       <c r="B45" t="s" s="17">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C45" t="s" s="18">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="D45" t="s" s="18">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="E45" t="s" s="18">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="F45" s="19"/>
     </row>
     <row r="46" ht="56.05" customHeight="1">
       <c r="A46" s="16"/>
       <c r="B46" t="s" s="17">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C46" t="s" s="18">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="D46" t="s" s="18">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="E46" t="s" s="18">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="F46" s="19"/>
     </row>
     <row r="47" ht="44.05" customHeight="1">
       <c r="A47" s="16"/>
       <c r="B47" t="s" s="17">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C47" t="s" s="18">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="D47" t="s" s="18">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="E47" t="s" s="18">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="F47" s="19"/>
     </row>
@@ -3147,16 +3173,16 @@
     <row r="49" ht="44.05" customHeight="1">
       <c r="A49" s="16"/>
       <c r="B49" t="s" s="17">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C49" t="s" s="18">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="D49" t="s" s="18">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="E49" t="s" s="18">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="F49" s="19"/>
     </row>
@@ -3171,86 +3197,86 @@
     <row r="51" ht="116.05" customHeight="1">
       <c r="A51" s="16"/>
       <c r="B51" t="s" s="17">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C51" t="s" s="18">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D51" t="s" s="18">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="E51" t="s" s="18">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="F51" t="s" s="18">
-        <v>124</v>
+        <v>128</v>
       </c>
     </row>
     <row r="52" ht="224.05" customHeight="1">
       <c r="A52" s="16"/>
       <c r="B52" t="s" s="17">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C52" t="s" s="18">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D52" t="s" s="18">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="E52" t="s" s="18">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="F52" t="s" s="18">
-        <v>126</v>
+        <v>130</v>
       </c>
     </row>
     <row r="53" ht="668.05" customHeight="1">
       <c r="A53" s="16"/>
       <c r="B53" t="s" s="17">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C53" t="s" s="18">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D53" t="s" s="18">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="E53" t="s" s="18">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="F53" t="s" s="18">
-        <v>126</v>
+        <v>130</v>
       </c>
     </row>
     <row r="54" ht="56.05" customHeight="1">
       <c r="A54" s="16"/>
       <c r="B54" t="s" s="17">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C54" t="s" s="18">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D54" t="s" s="18">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="E54" t="s" s="18">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="F54" s="19"/>
     </row>
     <row r="55" ht="44.05" customHeight="1">
       <c r="A55" s="16"/>
       <c r="B55" t="s" s="17">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C55" t="s" s="18">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="D55" t="s" s="18">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="E55" t="s" s="18">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="F55" s="19"/>
     </row>
@@ -3265,200 +3291,200 @@
     <row r="57" ht="56.05" customHeight="1">
       <c r="A57" s="16"/>
       <c r="B57" t="s" s="17">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C57" t="s" s="18">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="D57" t="s" s="18">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="E57" t="s" s="18">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="F57" s="19"/>
     </row>
     <row r="58" ht="44.05" customHeight="1">
       <c r="A58" s="16"/>
       <c r="B58" t="s" s="17">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C58" t="s" s="18">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="D58" t="s" s="18">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="E58" t="s" s="18">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="F58" s="19"/>
     </row>
     <row r="59" ht="92.05" customHeight="1">
       <c r="A59" s="16"/>
       <c r="B59" t="s" s="17">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C59" t="s" s="18">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="D59" t="s" s="18">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="E59" t="s" s="18">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="F59" s="19"/>
     </row>
     <row r="60" ht="56.05" customHeight="1">
       <c r="A60" s="16"/>
       <c r="B60" t="s" s="17">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C60" t="s" s="18">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="D60" t="s" s="18">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="E60" t="s" s="18">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="F60" t="s" s="18">
-        <v>142</v>
+        <v>146</v>
       </c>
     </row>
     <row r="61" ht="32.05" customHeight="1">
       <c r="A61" s="16"/>
       <c r="B61" t="s" s="17">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C61" t="s" s="18">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="D61" t="s" s="18">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="E61" t="s" s="18">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="F61" s="19"/>
     </row>
     <row r="62" ht="32.05" customHeight="1">
       <c r="A62" s="16"/>
       <c r="B62" t="s" s="17">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C62" t="s" s="18">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="D62" t="s" s="18">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="E62" t="s" s="18">
+        <v>150</v>
+      </c>
+      <c r="F62" t="s" s="18">
         <v>146</v>
-      </c>
-      <c r="F62" t="s" s="18">
-        <v>142</v>
       </c>
     </row>
     <row r="63" ht="32.05" customHeight="1">
       <c r="A63" s="16"/>
       <c r="B63" t="s" s="17">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C63" t="s" s="18">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="D63" t="s" s="18">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="E63" t="s" s="18">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="F63" t="s" s="18">
-        <v>142</v>
+        <v>146</v>
       </c>
     </row>
     <row r="64" ht="32.05" customHeight="1">
       <c r="A64" s="16"/>
       <c r="B64" t="s" s="17">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C64" t="s" s="18">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="D64" t="s" s="18">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="E64" t="s" s="18">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="F64" s="19"/>
     </row>
     <row r="65" ht="140.05" customHeight="1">
       <c r="A65" s="16"/>
       <c r="B65" t="s" s="17">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C65" t="s" s="18">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="D65" t="s" s="18">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="E65" t="s" s="18">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="F65" t="s" s="18">
-        <v>142</v>
+        <v>146</v>
       </c>
     </row>
     <row r="66" ht="92.05" customHeight="1">
       <c r="A66" s="16"/>
       <c r="B66" t="s" s="17">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C66" t="s" s="18">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="D66" t="s" s="18">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="E66" t="s" s="18">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="F66" s="19"/>
     </row>
     <row r="67" ht="44.05" customHeight="1">
       <c r="A67" s="16"/>
       <c r="B67" t="s" s="17">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C67" t="s" s="18">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="D67" t="s" s="18">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="E67" t="s" s="18">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="F67" s="19"/>
     </row>
     <row r="68" ht="116.05" customHeight="1">
       <c r="A68" s="16"/>
       <c r="B68" t="s" s="17">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C68" t="s" s="18">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="D68" t="s" s="18">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="E68" t="s" s="18">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="F68" s="19"/>
     </row>
@@ -3473,80 +3499,80 @@
     <row r="70" ht="68.05" customHeight="1">
       <c r="A70" s="16"/>
       <c r="B70" t="s" s="17">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="C70" t="s" s="18">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="D70" t="s" s="18">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="E70" t="s" s="18">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="F70" s="19"/>
     </row>
     <row r="71" ht="44.05" customHeight="1">
       <c r="A71" s="16"/>
       <c r="B71" t="s" s="17">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="C71" t="s" s="18">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="D71" t="s" s="18">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="E71" t="s" s="18">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="F71" s="19"/>
     </row>
     <row r="72" ht="44.05" customHeight="1">
       <c r="A72" s="16"/>
       <c r="B72" t="s" s="17">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="C72" t="s" s="18">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="D72" t="s" s="18">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="E72" t="s" s="18">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="F72" s="19"/>
     </row>
     <row r="73" ht="44.05" customHeight="1">
       <c r="A73" s="16"/>
       <c r="B73" t="s" s="17">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="C73" t="s" s="18">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="D73" t="s" s="18">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="E73" t="s" s="18">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="F73" s="19"/>
     </row>
     <row r="74" ht="56.05" customHeight="1">
       <c r="A74" s="16"/>
       <c r="B74" t="s" s="17">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="C74" t="s" s="18">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="D74" t="s" s="18">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="E74" t="s" s="18">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="F74" s="19"/>
     </row>
@@ -3561,32 +3587,32 @@
     <row r="76" ht="32.05" customHeight="1">
       <c r="A76" s="16"/>
       <c r="B76" t="s" s="17">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="C76" t="s" s="18">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="D76" t="s" s="18">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="E76" t="s" s="18">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="F76" s="19"/>
     </row>
     <row r="77" ht="56.05" customHeight="1">
       <c r="A77" s="16"/>
       <c r="B77" t="s" s="17">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="C77" t="s" s="18">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="D77" t="s" s="18">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="E77" t="s" s="18">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="F77" s="19"/>
     </row>
@@ -3601,114 +3627,114 @@
     <row r="79" ht="44.05" customHeight="1">
       <c r="A79" s="16"/>
       <c r="B79" t="s" s="17">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C79" t="s" s="18">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="D79" t="s" s="18">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="E79" t="s" s="18">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="F79" s="19"/>
     </row>
     <row r="80" ht="116.05" customHeight="1">
       <c r="A80" s="16"/>
       <c r="B80" t="s" s="17">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C80" t="s" s="18">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="D80" t="s" s="18">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="E80" t="s" s="18">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="F80" t="s" s="18">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="81" ht="116.05" customHeight="1">
       <c r="A81" s="16"/>
       <c r="B81" t="s" s="17">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C81" t="s" s="18">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="D81" t="s" s="18">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="E81" t="s" s="18">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="F81" s="19"/>
     </row>
     <row r="82" ht="128.05" customHeight="1">
       <c r="A82" s="16"/>
       <c r="B82" t="s" s="17">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C82" t="s" s="18">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="D82" t="s" s="18">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="E82" t="s" s="18">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="F82" s="19"/>
     </row>
     <row r="83" ht="56.05" customHeight="1">
       <c r="A83" s="16"/>
       <c r="B83" t="s" s="17">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C83" t="s" s="18">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="D83" t="s" s="18">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="E83" t="s" s="18">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="F83" s="19"/>
     </row>
     <row r="84" ht="92.05" customHeight="1">
       <c r="A84" s="16"/>
       <c r="B84" t="s" s="17">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C84" t="s" s="18">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="D84" t="s" s="18">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="E84" t="s" s="18">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="F84" s="19"/>
     </row>
     <row r="85" ht="44.05" customHeight="1">
       <c r="A85" s="16"/>
       <c r="B85" t="s" s="17">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C85" t="s" s="18">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="D85" t="s" s="18">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="E85" t="s" s="18">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="F85" s="19"/>
     </row>

</xml_diff>